<commit_message>
update sample templates downloads for HP Kayakalp-program
</commit_message>
<xml_diff>
--- a/components/download_templates/templates/Kayakalp_CH_DH_CHC_Excel_Import_Template.xlsx
+++ b/components/download_templates/templates/Kayakalp_CH_DH_CHC_Excel_Import_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\njo85\Desktop\Kayakalp formats\Kayakalp formats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\njo85\Desktop\Kayakalp Excel Import Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C5C30040-7D52-40AF-9487-06BC5FDC5BC0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4A25C7A-C234-4F61-9E96-11F0E0F7C253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D8962612-1CB3-4189-B3EC-736619A48D1E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D8962612-1CB3-4189-B3EC-736619A48D1E}"/>
   </bookViews>
   <sheets>
     <sheet name="CH DH CHC Quarterly Dataset" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,14 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -4631,8 +4639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB213EB5-9B3C-460D-94F1-741C123C3E90}">
   <dimension ref="A1:AZ425"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A412" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+      <selection activeCell="E416" sqref="E416"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4805,9 +4813,6 @@
         <v>0</v>
       </c>
       <c r="F10" s="10"/>
-      <c r="AZ10" s="6">
-        <v>3</v>
-      </c>
     </row>
     <row r="11" spans="1:52" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="19" t="s">
@@ -11359,8 +11364,8 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E9 E11:E15 E17:E21 E23:E27 E29:E33 E35:E39 E41:E45 E47:E51 E53:E57 E59:E63 E66:E70 E72:E76 E78:E82 E84:E88 E90:E94 E96:E100 E102:E106 E108:E112 E114:E118 E120:E124 E127:E131 E133:E137 E139:E143 E145:E149 E151:E155 E157:E161 E163:E167 E169:E173 E175:E179 E181:E185 E188:E192 E194:E198 E200:E204 E206:E210 E212:E216 E218:E222 E224:E228 E230:E234 E236:E240 E242:E246 E249:E253 E255:E259 E261:E265 E267:E271 E273:E277 E280:E284 E286:E290 E292:E296 E298:E302 E304:E308 E311:E315 E317:E321 E323:E327 E329:E333 E335:E339 E341:E345 E347:E351 E353:E357 E359:E363 E365:E369 E372:E381 E383:E392 E394:E403 E405:E414 E416:E425" xr:uid="{EBFB7FB8-CEAC-4B45-9400-AC51EA5A8C80}">
-      <formula1>$AZ$7:$AZ$10</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E9 E11:E15 E17:E21 E23:E27 E29:E33 E35:E39 E41:E45 E47:E51 E53:E57 E59:E63 E66:E70 E72:E76 E78:E82 E84:E88 E90:E94 E96:E100 E102:E106 E108:E112 E114:E118 E120:E124 E127:E131 E133:E137 E139:E143 E145:E149 E151:E155 E157:E161 E163:E167 E169:E173 E175:E179 E181:E185 E188:E192 E194:E198 E200:E204 E206:E210 E212:E216 E218:E222 E224:E228 E230:E234 E236:E240 E242:E246 E249:E253 E255:E259 E261:E265 E267:E271 E273:E277 E280:E284 E286:E290 E292:E296 E298:E302 E304:E308 E311:E315 E317:E321 E323:E327 E329:E333 E335:E339 E341:E345 E347:E351 E353:E357 E359:E363 E365:E369 E372:E381 E383:E392 E394:E403 E405:E414 E416:E425" xr:uid="{2B2CED72-3264-4FBA-9AF7-C40866451BC2}">
+      <formula1>$AZ$7:$AZ$9</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>